<commit_message>
wed attendace updated with absence counter
</commit_message>
<xml_diff>
--- a/Attendance/w12-14.xlsx
+++ b/Attendance/w12-14.xlsx
@@ -22,196 +22,196 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="65">
   <si>
+    <t xml:space="preserve">Neptun kód</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hiányzás</t>
+  </si>
+  <si>
     <t xml:space="preserve">Név</t>
   </si>
   <si>
-    <t xml:space="preserve">Neptun kód</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jelenlét</t>
+    <t xml:space="preserve">YXI8DJ</t>
   </si>
   <si>
     <t xml:space="preserve">Ferencsik Dorina Kinga</t>
   </si>
   <si>
-    <t xml:space="preserve">YXI8DJ</t>
-  </si>
-  <si>
     <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">363964489</t>
   </si>
   <si>
+    <t xml:space="preserve">K8HJGD</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gönczi Viktor</t>
   </si>
   <si>
-    <t xml:space="preserve">K8HJGD</t>
-  </si>
-  <si>
     <t xml:space="preserve">0</t>
   </si>
   <si>
     <t xml:space="preserve">308186307</t>
   </si>
   <si>
+    <t xml:space="preserve">ASL7ZK</t>
+  </si>
+  <si>
     <t xml:space="preserve">Horák Rajmund</t>
   </si>
   <si>
-    <t xml:space="preserve">ASL7ZK</t>
-  </si>
-  <si>
     <t xml:space="preserve">363968699</t>
   </si>
   <si>
+    <t xml:space="preserve">FWIY50</t>
+  </si>
+  <si>
     <t xml:space="preserve">Juhász Lilla</t>
   </si>
   <si>
-    <t xml:space="preserve">FWIY50</t>
-  </si>
-  <si>
     <t xml:space="preserve">336235073</t>
   </si>
   <si>
+    <t xml:space="preserve">KYDK4Z</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kása Dániel Zoltán</t>
   </si>
   <si>
-    <t xml:space="preserve">KYDK4Z</t>
-  </si>
-  <si>
     <t xml:space="preserve">363971197</t>
   </si>
   <si>
+    <t xml:space="preserve">PRSHNG</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kékedi Krisztián</t>
   </si>
   <si>
-    <t xml:space="preserve">PRSHNG</t>
-  </si>
-  <si>
     <t xml:space="preserve">308187960</t>
   </si>
   <si>
+    <t xml:space="preserve">UHV61T</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kiss Áron</t>
   </si>
   <si>
-    <t xml:space="preserve">UHV61T</t>
-  </si>
-  <si>
     <t xml:space="preserve">363972913</t>
   </si>
   <si>
+    <t xml:space="preserve">CDTD5F</t>
+  </si>
+  <si>
     <t xml:space="preserve">Makkai Márk</t>
   </si>
   <si>
-    <t xml:space="preserve">CDTD5F</t>
-  </si>
-  <si>
     <t xml:space="preserve">363975165</t>
   </si>
   <si>
+    <t xml:space="preserve">O60B05</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nagy Valter László</t>
   </si>
   <si>
-    <t xml:space="preserve">O60B05</t>
-  </si>
-  <si>
     <t xml:space="preserve">363960022</t>
   </si>
   <si>
+    <t xml:space="preserve">WLM9W8</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nussbaumer Alex</t>
   </si>
   <si>
-    <t xml:space="preserve">WLM9W8</t>
-  </si>
-  <si>
     <t xml:space="preserve">336236071</t>
   </si>
   <si>
+    <t xml:space="preserve">PXCZCK</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nyitrai Balázs</t>
   </si>
   <si>
-    <t xml:space="preserve">PXCZCK</t>
-  </si>
-  <si>
     <t xml:space="preserve">363968404</t>
   </si>
   <si>
+    <t xml:space="preserve">O1GLFP</t>
+  </si>
+  <si>
     <t xml:space="preserve">Papp Mihály</t>
   </si>
   <si>
-    <t xml:space="preserve">O1GLFP</t>
-  </si>
-  <si>
     <t xml:space="preserve">363960552</t>
   </si>
   <si>
+    <t xml:space="preserve">V6AP37</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pásztor Bence</t>
   </si>
   <si>
-    <t xml:space="preserve">V6AP37</t>
-  </si>
-  <si>
     <t xml:space="preserve">363960649</t>
   </si>
   <si>
+    <t xml:space="preserve">GCFA4K</t>
+  </si>
+  <si>
     <t xml:space="preserve">Putnóczki Fanni</t>
   </si>
   <si>
-    <t xml:space="preserve">GCFA4K</t>
-  </si>
-  <si>
     <t xml:space="preserve">363965773</t>
   </si>
   <si>
+    <t xml:space="preserve">MDBAFO</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sajó András</t>
   </si>
   <si>
-    <t xml:space="preserve">MDBAFO</t>
-  </si>
-  <si>
     <t xml:space="preserve">363969286</t>
   </si>
   <si>
+    <t xml:space="preserve">D7ITL3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Süle Ábel</t>
   </si>
   <si>
-    <t xml:space="preserve">D7ITL3</t>
-  </si>
-  <si>
     <t xml:space="preserve">363961661</t>
   </si>
   <si>
+    <t xml:space="preserve">G0XXTC</t>
+  </si>
+  <si>
     <t xml:space="preserve">Szacsuri Norbert</t>
   </si>
   <si>
-    <t xml:space="preserve">G0XXTC</t>
-  </si>
-  <si>
     <t xml:space="preserve">363967552</t>
   </si>
   <si>
+    <t xml:space="preserve">BB89VX</t>
+  </si>
+  <si>
     <t xml:space="preserve">Szemán Balázs</t>
   </si>
   <si>
-    <t xml:space="preserve">BB89VX</t>
-  </si>
-  <si>
     <t xml:space="preserve">363970592</t>
   </si>
   <si>
+    <t xml:space="preserve">AZCTJJ</t>
+  </si>
+  <si>
     <t xml:space="preserve">Szeszák Ádám</t>
   </si>
   <si>
-    <t xml:space="preserve">AZCTJJ</t>
-  </si>
-  <si>
     <t xml:space="preserve">336240453</t>
   </si>
   <si>
+    <t xml:space="preserve">M6N0DP</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vass Dávid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M6N0DP</t>
   </si>
   <si>
     <t xml:space="preserve">363958230</t>
@@ -226,7 +226,7 @@
     <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -256,6 +256,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -313,12 +320,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -338,7 +349,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -422,14 +437,14 @@
   <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
+      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="0" width="11.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="9" style="0" width="11.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="17" style="0" width="8.51"/>
@@ -441,550 +456,610 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="n">
+      <c r="D1" s="3" t="n">
         <v>43355</v>
       </c>
-      <c r="E1" s="2" t="n">
+      <c r="E1" s="3" t="n">
         <v>43369</v>
       </c>
-      <c r="F1" s="2" t="n">
+      <c r="F1" s="3" t="n">
         <v>43376</v>
       </c>
-      <c r="G1" s="2" t="n">
+      <c r="G1" s="3" t="n">
         <v>43383</v>
       </c>
-      <c r="H1" s="2" t="n">
+      <c r="H1" s="3" t="n">
         <v>43390</v>
       </c>
-      <c r="I1" s="3" t="n">
+      <c r="I1" s="4" t="n">
         <v>43397</v>
       </c>
-      <c r="J1" s="3" t="n">
+      <c r="J1" s="4" t="n">
         <v>43404</v>
       </c>
-      <c r="K1" s="3" t="n">
+      <c r="K1" s="4" t="n">
         <v>43411</v>
       </c>
-      <c r="L1" s="3" t="n">
+      <c r="L1" s="4" t="n">
         <v>43418</v>
       </c>
-      <c r="M1" s="3" t="n">
+      <c r="M1" s="4" t="n">
         <v>43425</v>
       </c>
-      <c r="N1" s="3" t="n">
+      <c r="N1" s="4" t="n">
         <v>43432</v>
       </c>
-      <c r="O1" s="3" t="n">
+      <c r="O1" s="4" t="n">
         <v>43439</v>
       </c>
-      <c r="P1" s="3" t="n">
+      <c r="P1" s="4" t="n">
         <v>43446</v>
       </c>
-      <c r="W1" s="4"/>
+      <c r="W1" s="5"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D2:I2,"0")&gt;4,"aláírás megtagadva", COUNTIF(D2:I2, "0"))</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="Q2" s="6" t="n">
+      <c r="D2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="Q2" s="8" t="n">
         <f aca="false">COUNTIF(D2:P2,"1")</f>
         <v>2</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D3:I3,"0")&gt;4,"aláírás megtagadva", COUNTIF(D3:I3, "0"))</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="Q3" s="6" t="n">
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="Q3" s="8" t="n">
         <f aca="false">COUNTIF(D3:P3,"1")</f>
         <v>1</v>
       </c>
-      <c r="W3" s="4" t="s">
+      <c r="W3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D4:I4,"0")&gt;4,"aláírás megtagadva", COUNTIF(D4:I4, "0"))</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="Q4" s="6" t="n">
+      <c r="D4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="Q4" s="8" t="n">
         <f aca="false">COUNTIF(D4:P4,"1")</f>
         <v>2</v>
       </c>
-      <c r="W4" s="4" t="s">
+      <c r="W4" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D5:I5,"0")&gt;4,"aláírás megtagadva", COUNTIF(D5:I5, "0"))</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="Q5" s="6" t="n">
+      <c r="D5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="Q5" s="8" t="n">
         <f aca="false">COUNTIF(D5:P5,"1")</f>
         <v>2</v>
       </c>
-      <c r="W5" s="4" t="s">
+      <c r="W5" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D6:I6,"0")&gt;4,"aláírás megtagadva", COUNTIF(D6:I6, "0"))</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="Q6" s="6" t="n">
+      <c r="D6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="Q6" s="8" t="n">
         <f aca="false">COUNTIF(D6:P6,"1")</f>
         <v>2</v>
       </c>
-      <c r="W6" s="4" t="s">
+      <c r="W6" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D7:I7,"0")&gt;4,"aláírás megtagadva", COUNTIF(D7:I7, "0"))</f>
+        <v>0</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="Q7" s="6" t="n">
+      <c r="D7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="Q7" s="8" t="n">
         <f aca="false">COUNTIF(D7:P7,"1")</f>
         <v>2</v>
       </c>
-      <c r="W7" s="4" t="s">
+      <c r="W7" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D8:I8,"0")&gt;4,"aláírás megtagadva", COUNTIF(D8:I8, "0"))</f>
+        <v>1</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="Q8" s="6" t="n">
+      <c r="E8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="Q8" s="8" t="n">
         <f aca="false">COUNTIF(D8:P8,"1")</f>
         <v>1</v>
       </c>
-      <c r="W8" s="4" t="s">
+      <c r="W8" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D9:I9,"0")&gt;4,"aláírás megtagadva", COUNTIF(D9:I9, "0"))</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="Q9" s="6" t="n">
+      <c r="D9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="Q9" s="8" t="n">
         <f aca="false">COUNTIF(D9:P9,"1")</f>
         <v>2</v>
       </c>
-      <c r="W9" s="4" t="s">
+      <c r="W9" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D10:I10,"0")&gt;4,"aláírás megtagadva", COUNTIF(D10:I10, "0"))</f>
+        <v>0</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="Q10" s="6" t="n">
+      <c r="D10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="Q10" s="8" t="n">
         <f aca="false">COUNTIF(D10:P10,"1")</f>
         <v>2</v>
       </c>
-      <c r="W10" s="4" t="s">
+      <c r="W10" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D11:I11,"0")&gt;4,"aláírás megtagadva", COUNTIF(D11:I11, "0"))</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="Q11" s="6" t="n">
+      <c r="D11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="Q11" s="8" t="n">
         <f aca="false">COUNTIF(D11:P11,"1")</f>
         <v>2</v>
       </c>
-      <c r="W11" s="4" t="s">
+      <c r="W11" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D12:I12,"0")&gt;4,"aláírás megtagadva", COUNTIF(D12:I12, "0"))</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="Q12" s="6" t="n">
+      <c r="D12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="Q12" s="8" t="n">
         <f aca="false">COUNTIF(D12:P12,"1")</f>
         <v>2</v>
       </c>
-      <c r="W12" s="4" t="s">
+      <c r="W12" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D13:I13,"0")&gt;4,"aláírás megtagadva", COUNTIF(D13:I13, "0"))</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="Q13" s="6" t="n">
+      <c r="D13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="Q13" s="8" t="n">
         <f aca="false">COUNTIF(D13:P13,"1")</f>
         <v>2</v>
       </c>
-      <c r="W13" s="4" t="s">
+      <c r="W13" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D14:I14,"0")&gt;4,"aláírás megtagadva", COUNTIF(D14:I14, "0"))</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="Q14" s="6" t="n">
+      <c r="D14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="Q14" s="8" t="n">
         <f aca="false">COUNTIF(D14:P14,"1")</f>
         <v>2</v>
       </c>
-      <c r="W14" s="4" t="s">
+      <c r="W14" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D15:I15,"0")&gt;4,"aláírás megtagadva", COUNTIF(D15:I15, "0"))</f>
+        <v>1</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="Q15" s="6" t="n">
+      <c r="E15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="Q15" s="8" t="n">
         <f aca="false">COUNTIF(D15:P15,"1")</f>
         <v>1</v>
       </c>
-      <c r="W15" s="4" t="s">
+      <c r="W15" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D16:I16,"0")&gt;4,"aláírás megtagadva", COUNTIF(D16:I16, "0"))</f>
+        <v>0</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="Q16" s="6" t="n">
+      <c r="D16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="Q16" s="8" t="n">
         <f aca="false">COUNTIF(D16:P16,"1")</f>
         <v>2</v>
       </c>
-      <c r="W16" s="4" t="s">
+      <c r="W16" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D17:I17,"0")&gt;4,"aláírás megtagadva", COUNTIF(D17:I17, "0"))</f>
+        <v>0</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="Q17" s="6" t="n">
+      <c r="D17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="Q17" s="8" t="n">
         <f aca="false">COUNTIF(D17:P17,"1")</f>
         <v>2</v>
       </c>
-      <c r="W17" s="4" t="s">
+      <c r="W17" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D18:I18,"0")&gt;4,"aláírás megtagadva", COUNTIF(D18:I18, "0"))</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="Q18" s="6" t="n">
+      <c r="D18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="Q18" s="8" t="n">
         <f aca="false">COUNTIF(D18:P18,"1")</f>
         <v>2</v>
       </c>
-      <c r="W18" s="4" t="s">
+      <c r="W18" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D19:I19,"0")&gt;4,"aláírás megtagadva", COUNTIF(D19:I19, "0"))</f>
+        <v>1</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="Q19" s="6" t="n">
+      <c r="E19" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="Q19" s="8" t="n">
         <f aca="false">COUNTIF(D19:P19,"1")</f>
         <v>1</v>
       </c>
-      <c r="W19" s="4" t="s">
+      <c r="W19" s="5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D20:I20,"0")&gt;4,"aláírás megtagadva", COUNTIF(D20:I20, "0"))</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="Q20" s="6" t="n">
+      <c r="D20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="Q20" s="8" t="n">
         <f aca="false">COUNTIF(D20:P20,"1")</f>
         <v>2</v>
       </c>
-      <c r="W20" s="4" t="s">
+      <c r="W20" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="7" t="n">
+        <f aca="false">IF(COUNTIF(D21:I21,"0")&gt;4,"aláírás megtagadva", COUNTIF(D21:I21, "0"))</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="Q21" s="6" t="n">
+      <c r="D21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="Q21" s="8" t="n">
         <f aca="false">COUNTIF(D21:P21,"1")</f>
         <v>2</v>
       </c>
-      <c r="W21" s="4" t="s">
+      <c r="W21" s="5" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>